<commit_message>
Updated with topics of July
</commit_message>
<xml_diff>
--- a/TimeSeries.xlsx
+++ b/TimeSeries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b0612544\Documents\Projects\Quality\Reports\June\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b0612544\Documents\Projects\Quality\Reports\July\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC25B8E3-F6B3-401D-93ED-8EC64B65D038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B67B9E-E653-41D6-A0FA-59CE19AE7CF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A1E6076-90AD-4A32-9861-A99DFFB6F447}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7A1E6076-90AD-4A32-9861-A99DFFB6F447}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Jun, 2021</t>
+  </si>
+  <si>
+    <t>Jul, 2021</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012BFEAD-AEFF-4BF6-9C64-73BB433DFCFE}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +841,17 @@
         <v>239</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>501</v>
+      </c>
+      <c r="C32">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>